<commit_message>
Welelelele de corrigir de acordo com o relatório, bye bye Transações
</commit_message>
<xml_diff>
--- a/documentos/GantBD.xlsx
+++ b/documentos/GantBD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\Desktop\TUDO\UNI\3 ANO\LI4\online-auctions\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E186A62B-3681-4F77-BB23-71BDBD56E411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0219F498-DADC-441F-9CB4-9640F4B940CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Project Management Templates</t>
   </si>
@@ -216,6 +216,27 @@
   </si>
   <si>
     <t>5.2 Caracterização das interfaces</t>
+  </si>
+  <si>
+    <t>3. Implementação da Solução</t>
+  </si>
+  <si>
+    <t>3.1 Implementação da BD</t>
+  </si>
+  <si>
+    <t>3.2 Desenho das Interfaces</t>
+  </si>
+  <si>
+    <t>3.5 Teste e Validação da Aplicação</t>
+  </si>
+  <si>
+    <t>3.6 Documentação</t>
+  </si>
+  <si>
+    <t>3.3 Desenvolvimento da Lógica de Negócio</t>
+  </si>
+  <si>
+    <t>3.4 Desenvolvimento das Interfaces</t>
   </si>
 </sst>
 </file>
@@ -984,6 +1005,9 @@
     <xf numFmtId="164" fontId="4" fillId="19" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -998,9 +1022,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1561,9 +1582,9 @@
   </sheetPr>
   <dimension ref="A1:DJ59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BP21" sqref="BP21"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AF47" sqref="AF47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,19 +1604,34 @@
     <col min="15" max="15" width="2.85546875" customWidth="1"/>
     <col min="16" max="19" width="3.140625" customWidth="1"/>
     <col min="20" max="21" width="2.85546875" customWidth="1"/>
-    <col min="22" max="22" width="2.42578125" customWidth="1"/>
-    <col min="23" max="40" width="2.5703125" customWidth="1"/>
+    <col min="22" max="23" width="3.42578125" customWidth="1"/>
+    <col min="24" max="24" width="3.5703125" customWidth="1"/>
+    <col min="25" max="25" width="3.42578125" customWidth="1"/>
+    <col min="26" max="26" width="2.85546875" customWidth="1"/>
+    <col min="27" max="40" width="2.5703125" customWidth="1"/>
     <col min="41" max="41" width="2.85546875" customWidth="1"/>
     <col min="42" max="42" width="2.5703125" customWidth="1"/>
     <col min="43" max="43" width="2.85546875" customWidth="1"/>
     <col min="44" max="44" width="3.28515625" customWidth="1"/>
-    <col min="45" max="46" width="2.85546875" customWidth="1"/>
+    <col min="45" max="45" width="2.85546875" customWidth="1"/>
+    <col min="46" max="46" width="3.7109375" customWidth="1"/>
     <col min="47" max="48" width="3.140625" customWidth="1"/>
-    <col min="49" max="50" width="2.85546875" customWidth="1"/>
-    <col min="51" max="51" width="3.42578125" customWidth="1"/>
-    <col min="52" max="71" width="2.5703125" customWidth="1"/>
+    <col min="49" max="49" width="3.28515625" customWidth="1"/>
+    <col min="50" max="50" width="3" customWidth="1"/>
+    <col min="51" max="52" width="3.42578125" customWidth="1"/>
+    <col min="53" max="53" width="3.5703125" customWidth="1"/>
+    <col min="54" max="54" width="3.42578125" customWidth="1"/>
+    <col min="55" max="56" width="3.140625" customWidth="1"/>
+    <col min="57" max="71" width="2.5703125" customWidth="1"/>
     <col min="72" max="72" width="3.28515625" customWidth="1"/>
-    <col min="73" max="113" width="2.5703125" customWidth="1"/>
+    <col min="73" max="76" width="2.5703125" customWidth="1"/>
+    <col min="77" max="77" width="3.42578125" customWidth="1"/>
+    <col min="78" max="78" width="2.5703125" customWidth="1"/>
+    <col min="79" max="79" width="3.42578125" customWidth="1"/>
+    <col min="80" max="80" width="3.28515625" customWidth="1"/>
+    <col min="81" max="81" width="3.42578125" customWidth="1"/>
+    <col min="82" max="82" width="3.140625" customWidth="1"/>
+    <col min="83" max="113" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:113" ht="28.5" x14ac:dyDescent="0.45">
@@ -1608,24 +1644,24 @@
       <c r="F1" s="80"/>
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="115"/>
-      <c r="V1" s="115"/>
-      <c r="W1" s="115"/>
-      <c r="X1" s="115"/>
-      <c r="Y1" s="115"/>
-      <c r="Z1" s="115"/>
-      <c r="AA1" s="115"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="110"/>
+      <c r="L1" s="110"/>
+      <c r="M1" s="110"/>
+      <c r="N1" s="110"/>
+      <c r="O1" s="110"/>
+      <c r="P1" s="110"/>
+      <c r="Q1" s="110"/>
+      <c r="R1" s="110"/>
+      <c r="S1" s="110"/>
+      <c r="T1" s="110"/>
+      <c r="U1" s="110"/>
+      <c r="V1" s="110"/>
+      <c r="W1" s="110"/>
+      <c r="X1" s="110"/>
+      <c r="Y1" s="110"/>
+      <c r="Z1" s="110"/>
+      <c r="AA1" s="110"/>
     </row>
     <row r="2" spans="1:113" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
@@ -1634,10 +1670,10 @@
       <c r="D2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="113">
-        <v>45187</v>
-      </c>
-      <c r="F2" s="114"/>
+      <c r="E2" s="114">
+        <v>45243</v>
+      </c>
+      <c r="F2" s="115"/>
     </row>
     <row r="3" spans="1:113" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
@@ -1646,10 +1682,10 @@
       <c r="D3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="113">
-        <v>45149</v>
-      </c>
-      <c r="F3" s="114"/>
+      <c r="E3" s="114">
+        <v>45315</v>
+      </c>
+      <c r="F3" s="115"/>
     </row>
     <row r="4" spans="1:113" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="6" t="s">
@@ -1658,579 +1694,579 @@
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="110">
+      <c r="I4" s="111">
         <f>I5</f>
-        <v>45187</v>
-      </c>
-      <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="111"/>
-      <c r="M4" s="111"/>
-      <c r="N4" s="111"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="110">
+        <v>45243</v>
+      </c>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="113"/>
+      <c r="P4" s="111">
         <f>P5</f>
-        <v>45194</v>
-      </c>
-      <c r="Q4" s="111"/>
-      <c r="R4" s="111"/>
-      <c r="S4" s="111"/>
-      <c r="T4" s="111"/>
-      <c r="U4" s="111"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="110">
+        <v>45250</v>
+      </c>
+      <c r="Q4" s="112"/>
+      <c r="R4" s="112"/>
+      <c r="S4" s="112"/>
+      <c r="T4" s="112"/>
+      <c r="U4" s="112"/>
+      <c r="V4" s="113"/>
+      <c r="W4" s="111">
         <f>W5</f>
-        <v>45201</v>
-      </c>
-      <c r="X4" s="111"/>
-      <c r="Y4" s="111"/>
-      <c r="Z4" s="111"/>
-      <c r="AA4" s="111"/>
-      <c r="AB4" s="111"/>
-      <c r="AC4" s="112"/>
-      <c r="AD4" s="110">
+        <v>45257</v>
+      </c>
+      <c r="X4" s="112"/>
+      <c r="Y4" s="112"/>
+      <c r="Z4" s="112"/>
+      <c r="AA4" s="112"/>
+      <c r="AB4" s="112"/>
+      <c r="AC4" s="113"/>
+      <c r="AD4" s="111">
         <f>AD5</f>
-        <v>45208</v>
-      </c>
-      <c r="AE4" s="111"/>
-      <c r="AF4" s="111"/>
-      <c r="AG4" s="111"/>
-      <c r="AH4" s="111"/>
-      <c r="AI4" s="111"/>
-      <c r="AJ4" s="112"/>
-      <c r="AK4" s="110">
+        <v>45264</v>
+      </c>
+      <c r="AE4" s="112"/>
+      <c r="AF4" s="112"/>
+      <c r="AG4" s="112"/>
+      <c r="AH4" s="112"/>
+      <c r="AI4" s="112"/>
+      <c r="AJ4" s="113"/>
+      <c r="AK4" s="111">
         <f>AK5</f>
-        <v>45215</v>
-      </c>
-      <c r="AL4" s="111"/>
-      <c r="AM4" s="111"/>
-      <c r="AN4" s="111"/>
-      <c r="AO4" s="111"/>
-      <c r="AP4" s="111"/>
-      <c r="AQ4" s="112"/>
-      <c r="AR4" s="110">
+        <v>45271</v>
+      </c>
+      <c r="AL4" s="112"/>
+      <c r="AM4" s="112"/>
+      <c r="AN4" s="112"/>
+      <c r="AO4" s="112"/>
+      <c r="AP4" s="112"/>
+      <c r="AQ4" s="113"/>
+      <c r="AR4" s="111">
         <f>AR5</f>
-        <v>45222</v>
-      </c>
-      <c r="AS4" s="111"/>
-      <c r="AT4" s="111"/>
-      <c r="AU4" s="111"/>
-      <c r="AV4" s="111"/>
-      <c r="AW4" s="111"/>
-      <c r="AX4" s="112"/>
-      <c r="AY4" s="110">
+        <v>45278</v>
+      </c>
+      <c r="AS4" s="112"/>
+      <c r="AT4" s="112"/>
+      <c r="AU4" s="112"/>
+      <c r="AV4" s="112"/>
+      <c r="AW4" s="112"/>
+      <c r="AX4" s="113"/>
+      <c r="AY4" s="111">
         <f>AY5</f>
-        <v>45229</v>
-      </c>
-      <c r="AZ4" s="111"/>
-      <c r="BA4" s="111"/>
-      <c r="BB4" s="111"/>
-      <c r="BC4" s="111"/>
-      <c r="BD4" s="111"/>
-      <c r="BE4" s="112"/>
-      <c r="BF4" s="110">
+        <v>45285</v>
+      </c>
+      <c r="AZ4" s="112"/>
+      <c r="BA4" s="112"/>
+      <c r="BB4" s="112"/>
+      <c r="BC4" s="112"/>
+      <c r="BD4" s="112"/>
+      <c r="BE4" s="113"/>
+      <c r="BF4" s="111">
         <f>BF5</f>
-        <v>45236</v>
-      </c>
-      <c r="BG4" s="111"/>
-      <c r="BH4" s="111"/>
-      <c r="BI4" s="111"/>
-      <c r="BJ4" s="111"/>
-      <c r="BK4" s="111"/>
-      <c r="BL4" s="112"/>
-      <c r="BM4" s="110">
+        <v>45292</v>
+      </c>
+      <c r="BG4" s="112"/>
+      <c r="BH4" s="112"/>
+      <c r="BI4" s="112"/>
+      <c r="BJ4" s="112"/>
+      <c r="BK4" s="112"/>
+      <c r="BL4" s="113"/>
+      <c r="BM4" s="111">
         <f>BM5</f>
-        <v>45243</v>
-      </c>
-      <c r="BN4" s="111"/>
-      <c r="BO4" s="111"/>
-      <c r="BP4" s="111"/>
-      <c r="BQ4" s="111"/>
-      <c r="BR4" s="111"/>
-      <c r="BS4" s="112"/>
-      <c r="BT4" s="110">
+        <v>45299</v>
+      </c>
+      <c r="BN4" s="112"/>
+      <c r="BO4" s="112"/>
+      <c r="BP4" s="112"/>
+      <c r="BQ4" s="112"/>
+      <c r="BR4" s="112"/>
+      <c r="BS4" s="113"/>
+      <c r="BT4" s="111">
         <f>BT5</f>
-        <v>45250</v>
-      </c>
-      <c r="BU4" s="111"/>
-      <c r="BV4" s="111"/>
-      <c r="BW4" s="111"/>
-      <c r="BX4" s="111"/>
-      <c r="BY4" s="111"/>
-      <c r="BZ4" s="112"/>
-      <c r="CA4" s="110">
+        <v>45306</v>
+      </c>
+      <c r="BU4" s="112"/>
+      <c r="BV4" s="112"/>
+      <c r="BW4" s="112"/>
+      <c r="BX4" s="112"/>
+      <c r="BY4" s="112"/>
+      <c r="BZ4" s="113"/>
+      <c r="CA4" s="111">
         <f>CA5</f>
-        <v>45257</v>
-      </c>
-      <c r="CB4" s="111"/>
-      <c r="CC4" s="111"/>
-      <c r="CD4" s="111"/>
-      <c r="CE4" s="111"/>
-      <c r="CF4" s="111"/>
-      <c r="CG4" s="112"/>
-      <c r="CH4" s="110">
+        <v>45313</v>
+      </c>
+      <c r="CB4" s="112"/>
+      <c r="CC4" s="112"/>
+      <c r="CD4" s="112"/>
+      <c r="CE4" s="112"/>
+      <c r="CF4" s="112"/>
+      <c r="CG4" s="113"/>
+      <c r="CH4" s="111">
         <f>CH5</f>
-        <v>45264</v>
-      </c>
-      <c r="CI4" s="111"/>
-      <c r="CJ4" s="111"/>
-      <c r="CK4" s="111"/>
-      <c r="CL4" s="111"/>
-      <c r="CM4" s="111"/>
-      <c r="CN4" s="112"/>
-      <c r="CO4" s="110">
+        <v>45320</v>
+      </c>
+      <c r="CI4" s="112"/>
+      <c r="CJ4" s="112"/>
+      <c r="CK4" s="112"/>
+      <c r="CL4" s="112"/>
+      <c r="CM4" s="112"/>
+      <c r="CN4" s="113"/>
+      <c r="CO4" s="111">
         <f>CO5</f>
-        <v>45271</v>
-      </c>
-      <c r="CP4" s="111"/>
-      <c r="CQ4" s="111"/>
-      <c r="CR4" s="111"/>
-      <c r="CS4" s="111"/>
-      <c r="CT4" s="111"/>
-      <c r="CU4" s="112"/>
-      <c r="CV4" s="110">
+        <v>45327</v>
+      </c>
+      <c r="CP4" s="112"/>
+      <c r="CQ4" s="112"/>
+      <c r="CR4" s="112"/>
+      <c r="CS4" s="112"/>
+      <c r="CT4" s="112"/>
+      <c r="CU4" s="113"/>
+      <c r="CV4" s="111">
         <f>CV5</f>
-        <v>45278</v>
-      </c>
-      <c r="CW4" s="111"/>
-      <c r="CX4" s="111"/>
-      <c r="CY4" s="111"/>
-      <c r="CZ4" s="111"/>
-      <c r="DA4" s="111"/>
-      <c r="DB4" s="112"/>
-      <c r="DC4" s="110">
+        <v>45334</v>
+      </c>
+      <c r="CW4" s="112"/>
+      <c r="CX4" s="112"/>
+      <c r="CY4" s="112"/>
+      <c r="CZ4" s="112"/>
+      <c r="DA4" s="112"/>
+      <c r="DB4" s="113"/>
+      <c r="DC4" s="111">
         <f>DC5</f>
-        <v>45285</v>
-      </c>
-      <c r="DD4" s="111"/>
-      <c r="DE4" s="111"/>
-      <c r="DF4" s="111"/>
-      <c r="DG4" s="111"/>
-      <c r="DH4" s="111"/>
-      <c r="DI4" s="112"/>
+        <v>45341</v>
+      </c>
+      <c r="DD4" s="112"/>
+      <c r="DE4" s="112"/>
+      <c r="DF4" s="112"/>
+      <c r="DG4" s="112"/>
+      <c r="DH4" s="112"/>
+      <c r="DI4" s="113"/>
     </row>
     <row r="5" spans="1:113" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="G5" s="6"/>
       <c r="I5" s="13">
         <f>E2-WEEKDAY(E2,1)+2+7*(E4-1)</f>
-        <v>45187</v>
+        <v>45243</v>
       </c>
       <c r="J5" s="12">
         <f>I5+1</f>
-        <v>45188</v>
+        <v>45244</v>
       </c>
       <c r="K5" s="12">
         <f>J5+1</f>
-        <v>45189</v>
+        <v>45245</v>
       </c>
       <c r="L5" s="12">
-        <f t="shared" ref="K5:AX5" si="0">K5+1</f>
-        <v>45190</v>
+        <f t="shared" ref="L5:AX5" si="0">K5+1</f>
+        <v>45246</v>
       </c>
       <c r="M5" s="12">
         <f t="shared" si="0"/>
-        <v>45191</v>
+        <v>45247</v>
       </c>
       <c r="N5" s="12">
         <f t="shared" si="0"/>
-        <v>45192</v>
+        <v>45248</v>
       </c>
       <c r="O5" s="14">
         <f t="shared" si="0"/>
-        <v>45193</v>
+        <v>45249</v>
       </c>
       <c r="P5" s="13">
         <f>O5+1</f>
-        <v>45194</v>
+        <v>45250</v>
       </c>
       <c r="Q5" s="12">
         <f>P5+1</f>
-        <v>45195</v>
+        <v>45251</v>
       </c>
       <c r="R5" s="12">
         <f t="shared" si="0"/>
-        <v>45196</v>
+        <v>45252</v>
       </c>
       <c r="S5" s="12">
         <f t="shared" si="0"/>
-        <v>45197</v>
+        <v>45253</v>
       </c>
       <c r="T5" s="12">
         <f t="shared" si="0"/>
-        <v>45198</v>
+        <v>45254</v>
       </c>
       <c r="U5" s="12">
         <f t="shared" si="0"/>
-        <v>45199</v>
+        <v>45255</v>
       </c>
       <c r="V5" s="14">
         <f t="shared" si="0"/>
-        <v>45200</v>
+        <v>45256</v>
       </c>
       <c r="W5" s="13">
         <f>V5+1</f>
-        <v>45201</v>
+        <v>45257</v>
       </c>
       <c r="X5" s="12">
         <f>W5+1</f>
-        <v>45202</v>
+        <v>45258</v>
       </c>
       <c r="Y5" s="12">
         <f t="shared" si="0"/>
-        <v>45203</v>
+        <v>45259</v>
       </c>
       <c r="Z5" s="12">
         <f t="shared" si="0"/>
-        <v>45204</v>
+        <v>45260</v>
       </c>
       <c r="AA5" s="12">
         <f t="shared" si="0"/>
-        <v>45205</v>
+        <v>45261</v>
       </c>
       <c r="AB5" s="12">
         <f t="shared" si="0"/>
-        <v>45206</v>
+        <v>45262</v>
       </c>
       <c r="AC5" s="14">
         <f t="shared" si="0"/>
-        <v>45207</v>
+        <v>45263</v>
       </c>
       <c r="AD5" s="13">
         <f>AC5+1</f>
-        <v>45208</v>
+        <v>45264</v>
       </c>
       <c r="AE5" s="12">
         <f>AD5+1</f>
-        <v>45209</v>
+        <v>45265</v>
       </c>
       <c r="AF5" s="12">
         <f t="shared" si="0"/>
-        <v>45210</v>
+        <v>45266</v>
       </c>
       <c r="AG5" s="12">
         <f t="shared" si="0"/>
-        <v>45211</v>
+        <v>45267</v>
       </c>
       <c r="AH5" s="12">
         <f t="shared" si="0"/>
-        <v>45212</v>
+        <v>45268</v>
       </c>
       <c r="AI5" s="12">
         <f t="shared" si="0"/>
-        <v>45213</v>
+        <v>45269</v>
       </c>
       <c r="AJ5" s="14">
         <f t="shared" si="0"/>
-        <v>45214</v>
+        <v>45270</v>
       </c>
       <c r="AK5" s="13">
         <f>AJ5+1</f>
-        <v>45215</v>
+        <v>45271</v>
       </c>
       <c r="AL5" s="12">
         <f>AK5+1</f>
-        <v>45216</v>
+        <v>45272</v>
       </c>
       <c r="AM5" s="12">
         <f t="shared" si="0"/>
-        <v>45217</v>
+        <v>45273</v>
       </c>
       <c r="AN5" s="12">
         <f t="shared" si="0"/>
-        <v>45218</v>
+        <v>45274</v>
       </c>
       <c r="AO5" s="12">
         <f t="shared" si="0"/>
-        <v>45219</v>
+        <v>45275</v>
       </c>
       <c r="AP5" s="12">
         <f t="shared" si="0"/>
-        <v>45220</v>
+        <v>45276</v>
       </c>
       <c r="AQ5" s="14">
         <f t="shared" si="0"/>
-        <v>45221</v>
+        <v>45277</v>
       </c>
       <c r="AR5" s="13">
         <f>AQ5+1</f>
-        <v>45222</v>
+        <v>45278</v>
       </c>
       <c r="AS5" s="12">
         <f>AR5+1</f>
-        <v>45223</v>
+        <v>45279</v>
       </c>
       <c r="AT5" s="12">
         <f t="shared" si="0"/>
-        <v>45224</v>
+        <v>45280</v>
       </c>
       <c r="AU5" s="12">
         <f t="shared" si="0"/>
-        <v>45225</v>
+        <v>45281</v>
       </c>
       <c r="AV5" s="12">
         <f t="shared" si="0"/>
-        <v>45226</v>
+        <v>45282</v>
       </c>
       <c r="AW5" s="12">
         <f t="shared" si="0"/>
-        <v>45227</v>
+        <v>45283</v>
       </c>
       <c r="AX5" s="14">
         <f t="shared" si="0"/>
-        <v>45228</v>
+        <v>45284</v>
       </c>
       <c r="AY5" s="13">
         <f>AX5+1</f>
-        <v>45229</v>
+        <v>45285</v>
       </c>
       <c r="AZ5" s="12">
         <f>AY5+1</f>
-        <v>45230</v>
+        <v>45286</v>
       </c>
       <c r="BA5" s="12">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
-        <v>45231</v>
+        <v>45287</v>
       </c>
       <c r="BB5" s="12">
         <f t="shared" si="1"/>
-        <v>45232</v>
+        <v>45288</v>
       </c>
       <c r="BC5" s="12">
         <f t="shared" si="1"/>
-        <v>45233</v>
+        <v>45289</v>
       </c>
       <c r="BD5" s="12">
         <f t="shared" si="1"/>
-        <v>45234</v>
+        <v>45290</v>
       </c>
       <c r="BE5" s="14">
         <f t="shared" si="1"/>
-        <v>45235</v>
+        <v>45291</v>
       </c>
       <c r="BF5" s="13">
         <f>BE5+1</f>
-        <v>45236</v>
+        <v>45292</v>
       </c>
       <c r="BG5" s="12">
         <f>BF5+1</f>
-        <v>45237</v>
+        <v>45293</v>
       </c>
       <c r="BH5" s="12">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
-        <v>45238</v>
+        <v>45294</v>
       </c>
       <c r="BI5" s="12">
         <f t="shared" si="2"/>
-        <v>45239</v>
+        <v>45295</v>
       </c>
       <c r="BJ5" s="12">
         <f t="shared" si="2"/>
-        <v>45240</v>
+        <v>45296</v>
       </c>
       <c r="BK5" s="12">
         <f t="shared" si="2"/>
-        <v>45241</v>
+        <v>45297</v>
       </c>
       <c r="BL5" s="14">
         <f t="shared" si="2"/>
-        <v>45242</v>
+        <v>45298</v>
       </c>
       <c r="BM5" s="13">
         <f>BL5+1</f>
-        <v>45243</v>
+        <v>45299</v>
       </c>
       <c r="BN5" s="12">
         <f>BM5+1</f>
-        <v>45244</v>
+        <v>45300</v>
       </c>
       <c r="BO5" s="12">
         <f t="shared" ref="BO5" si="3">BN5+1</f>
-        <v>45245</v>
+        <v>45301</v>
       </c>
       <c r="BP5" s="12">
         <f t="shared" ref="BP5" si="4">BO5+1</f>
-        <v>45246</v>
+        <v>45302</v>
       </c>
       <c r="BQ5" s="12">
         <f t="shared" ref="BQ5" si="5">BP5+1</f>
-        <v>45247</v>
+        <v>45303</v>
       </c>
       <c r="BR5" s="12">
         <f t="shared" ref="BR5" si="6">BQ5+1</f>
-        <v>45248</v>
+        <v>45304</v>
       </c>
       <c r="BS5" s="14">
         <f t="shared" ref="BS5" si="7">BR5+1</f>
-        <v>45249</v>
+        <v>45305</v>
       </c>
       <c r="BT5" s="13">
         <f>BS5+1</f>
-        <v>45250</v>
+        <v>45306</v>
       </c>
       <c r="BU5" s="12">
         <f>BT5+1</f>
-        <v>45251</v>
+        <v>45307</v>
       </c>
       <c r="BV5" s="12">
         <f t="shared" ref="BV5" si="8">BU5+1</f>
-        <v>45252</v>
+        <v>45308</v>
       </c>
       <c r="BW5" s="12">
         <f t="shared" ref="BW5" si="9">BV5+1</f>
-        <v>45253</v>
+        <v>45309</v>
       </c>
       <c r="BX5" s="12">
         <f t="shared" ref="BX5" si="10">BW5+1</f>
-        <v>45254</v>
+        <v>45310</v>
       </c>
       <c r="BY5" s="12">
         <f t="shared" ref="BY5" si="11">BX5+1</f>
-        <v>45255</v>
+        <v>45311</v>
       </c>
       <c r="BZ5" s="14">
         <f t="shared" ref="BZ5" si="12">BY5+1</f>
-        <v>45256</v>
+        <v>45312</v>
       </c>
       <c r="CA5" s="13">
         <f>BZ5+1</f>
-        <v>45257</v>
+        <v>45313</v>
       </c>
       <c r="CB5" s="12">
         <f>CA5+1</f>
-        <v>45258</v>
+        <v>45314</v>
       </c>
       <c r="CC5" s="12">
         <f t="shared" ref="CC5" si="13">CB5+1</f>
-        <v>45259</v>
+        <v>45315</v>
       </c>
       <c r="CD5" s="12">
         <f t="shared" ref="CD5" si="14">CC5+1</f>
-        <v>45260</v>
+        <v>45316</v>
       </c>
       <c r="CE5" s="12">
         <f t="shared" ref="CE5" si="15">CD5+1</f>
-        <v>45261</v>
+        <v>45317</v>
       </c>
       <c r="CF5" s="12">
         <f t="shared" ref="CF5" si="16">CE5+1</f>
-        <v>45262</v>
+        <v>45318</v>
       </c>
       <c r="CG5" s="14">
         <f t="shared" ref="CG5" si="17">CF5+1</f>
-        <v>45263</v>
+        <v>45319</v>
       </c>
       <c r="CH5" s="13">
         <f>CG5+1</f>
-        <v>45264</v>
+        <v>45320</v>
       </c>
       <c r="CI5" s="12">
         <f>CH5+1</f>
-        <v>45265</v>
+        <v>45321</v>
       </c>
       <c r="CJ5" s="12">
         <f t="shared" ref="CJ5" si="18">CI5+1</f>
-        <v>45266</v>
+        <v>45322</v>
       </c>
       <c r="CK5" s="12">
         <f t="shared" ref="CK5" si="19">CJ5+1</f>
-        <v>45267</v>
+        <v>45323</v>
       </c>
       <c r="CL5" s="12">
         <f t="shared" ref="CL5" si="20">CK5+1</f>
-        <v>45268</v>
+        <v>45324</v>
       </c>
       <c r="CM5" s="12">
         <f t="shared" ref="CM5" si="21">CL5+1</f>
-        <v>45269</v>
+        <v>45325</v>
       </c>
       <c r="CN5" s="14">
         <f t="shared" ref="CN5" si="22">CM5+1</f>
-        <v>45270</v>
+        <v>45326</v>
       </c>
       <c r="CO5" s="13">
         <f>CN5+1</f>
-        <v>45271</v>
+        <v>45327</v>
       </c>
       <c r="CP5" s="12">
         <f>CO5+1</f>
-        <v>45272</v>
+        <v>45328</v>
       </c>
       <c r="CQ5" s="12">
         <f t="shared" ref="CQ5" si="23">CP5+1</f>
-        <v>45273</v>
+        <v>45329</v>
       </c>
       <c r="CR5" s="12">
         <f t="shared" ref="CR5" si="24">CQ5+1</f>
-        <v>45274</v>
+        <v>45330</v>
       </c>
       <c r="CS5" s="12">
         <f t="shared" ref="CS5" si="25">CR5+1</f>
-        <v>45275</v>
+        <v>45331</v>
       </c>
       <c r="CT5" s="12">
         <f t="shared" ref="CT5" si="26">CS5+1</f>
-        <v>45276</v>
+        <v>45332</v>
       </c>
       <c r="CU5" s="14">
         <f t="shared" ref="CU5" si="27">CT5+1</f>
-        <v>45277</v>
+        <v>45333</v>
       </c>
       <c r="CV5" s="13">
         <f>CU5+1</f>
-        <v>45278</v>
+        <v>45334</v>
       </c>
       <c r="CW5" s="12">
         <f>CV5+1</f>
-        <v>45279</v>
+        <v>45335</v>
       </c>
       <c r="CX5" s="12">
         <f t="shared" ref="CX5" si="28">CW5+1</f>
-        <v>45280</v>
+        <v>45336</v>
       </c>
       <c r="CY5" s="12">
         <f t="shared" ref="CY5" si="29">CX5+1</f>
-        <v>45281</v>
+        <v>45337</v>
       </c>
       <c r="CZ5" s="12">
         <f t="shared" ref="CZ5" si="30">CY5+1</f>
-        <v>45282</v>
+        <v>45338</v>
       </c>
       <c r="DA5" s="12">
         <f t="shared" ref="DA5" si="31">CZ5+1</f>
-        <v>45283</v>
+        <v>45339</v>
       </c>
       <c r="DB5" s="14">
         <f t="shared" ref="DB5" si="32">DA5+1</f>
-        <v>45284</v>
+        <v>45340</v>
       </c>
       <c r="DC5" s="13">
         <f>DB5+1</f>
-        <v>45285</v>
+        <v>45341</v>
       </c>
       <c r="DD5" s="12">
         <f>DC5+1</f>
-        <v>45286</v>
+        <v>45342</v>
       </c>
       <c r="DE5" s="12">
         <f t="shared" ref="DE5" si="33">DD5+1</f>
-        <v>45287</v>
+        <v>45343</v>
       </c>
       <c r="DF5" s="12">
         <f t="shared" ref="DF5" si="34">DE5+1</f>
-        <v>45288</v>
+        <v>45344</v>
       </c>
       <c r="DG5" s="12">
         <f t="shared" ref="DG5" si="35">DF5+1</f>
-        <v>45289</v>
+        <v>45345</v>
       </c>
       <c r="DH5" s="12">
         <f t="shared" ref="DH5" si="36">DG5+1</f>
-        <v>45290</v>
+        <v>45346</v>
       </c>
       <c r="DI5" s="14">
         <f t="shared" ref="DI5" si="37">DH5+1</f>
-        <v>45291</v>
+        <v>45347</v>
       </c>
     </row>
     <row r="6" spans="1:113" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5755,15 +5791,21 @@
     </row>
     <row r="32" spans="1:113" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
-      <c r="B32" s="58"/>
+      <c r="B32" s="58" t="s">
+        <v>46</v>
+      </c>
       <c r="C32" s="59"/>
       <c r="D32" s="60"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="62"/>
+      <c r="E32" s="61">
+        <v>45243</v>
+      </c>
+      <c r="F32" s="62">
+        <v>45315</v>
+      </c>
       <c r="G32" s="23"/>
-      <c r="H32" s="23" t="str">
+      <c r="H32" s="23">
         <f t="shared" si="46"/>
-        <v/>
+        <v>73</v>
       </c>
       <c r="I32" s="68"/>
       <c r="J32" s="68"/>
@@ -5873,15 +5915,21 @@
     </row>
     <row r="33" spans="1:114" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17"/>
-      <c r="B33" s="63"/>
+      <c r="B33" s="63" t="s">
+        <v>47</v>
+      </c>
       <c r="C33" s="64"/>
       <c r="D33" s="65"/>
-      <c r="E33" s="66"/>
-      <c r="F33" s="67"/>
+      <c r="E33" s="66">
+        <v>45243</v>
+      </c>
+      <c r="F33" s="67">
+        <v>45249</v>
+      </c>
       <c r="G33" s="23"/>
-      <c r="H33" s="23" t="str">
+      <c r="H33" s="23">
         <f t="shared" si="46"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="I33" s="68"/>
       <c r="J33" s="68"/>
@@ -5991,15 +6039,21 @@
     </row>
     <row r="34" spans="1:114" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17"/>
-      <c r="B34" s="63"/>
+      <c r="B34" s="63" t="s">
+        <v>48</v>
+      </c>
       <c r="C34" s="64"/>
       <c r="D34" s="65"/>
-      <c r="E34" s="66"/>
-      <c r="F34" s="67"/>
+      <c r="E34" s="66">
+        <v>45250</v>
+      </c>
+      <c r="F34" s="67">
+        <v>45256</v>
+      </c>
       <c r="G34" s="23"/>
-      <c r="H34" s="23" t="str">
+      <c r="H34" s="23">
         <f t="shared" si="46"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="I34" s="68"/>
       <c r="J34" s="68"/>
@@ -6109,15 +6163,21 @@
     </row>
     <row r="35" spans="1:114" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17"/>
-      <c r="B35" s="63"/>
+      <c r="B35" s="63" t="s">
+        <v>51</v>
+      </c>
       <c r="C35" s="64"/>
       <c r="D35" s="65"/>
-      <c r="E35" s="66"/>
-      <c r="F35" s="67"/>
+      <c r="E35" s="66">
+        <v>45257</v>
+      </c>
+      <c r="F35" s="67">
+        <v>45277</v>
+      </c>
       <c r="G35" s="23"/>
-      <c r="H35" s="23" t="str">
+      <c r="H35" s="23">
         <f t="shared" si="46"/>
-        <v/>
+        <v>21</v>
       </c>
       <c r="I35" s="68"/>
       <c r="J35" s="68"/>
@@ -6227,15 +6287,21 @@
     </row>
     <row r="36" spans="1:114" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17"/>
-      <c r="B36" s="63"/>
+      <c r="B36" s="63" t="s">
+        <v>52</v>
+      </c>
       <c r="C36" s="64"/>
       <c r="D36" s="65"/>
-      <c r="E36" s="66"/>
-      <c r="F36" s="67"/>
+      <c r="E36" s="66">
+        <v>45264</v>
+      </c>
+      <c r="F36" s="67">
+        <v>45284</v>
+      </c>
       <c r="G36" s="23"/>
-      <c r="H36" s="23" t="str">
+      <c r="H36" s="23">
         <f t="shared" si="46"/>
-        <v/>
+        <v>21</v>
       </c>
       <c r="I36" s="68"/>
       <c r="J36" s="68"/>
@@ -6345,15 +6411,21 @@
     </row>
     <row r="37" spans="1:114" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17"/>
-      <c r="B37" s="63"/>
+      <c r="B37" s="63" t="s">
+        <v>49</v>
+      </c>
       <c r="C37" s="64"/>
       <c r="D37" s="65"/>
-      <c r="E37" s="66"/>
-      <c r="F37" s="67"/>
+      <c r="E37" s="66">
+        <v>45293</v>
+      </c>
+      <c r="F37" s="67">
+        <v>45305</v>
+      </c>
       <c r="G37" s="23"/>
-      <c r="H37" s="23" t="str">
+      <c r="H37" s="23">
         <f t="shared" si="46"/>
-        <v/>
+        <v>13</v>
       </c>
       <c r="I37" s="68"/>
       <c r="J37" s="68"/>
@@ -6463,15 +6535,21 @@
     </row>
     <row r="38" spans="1:114" s="3" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17"/>
-      <c r="B38" s="63"/>
+      <c r="B38" s="63" t="s">
+        <v>50</v>
+      </c>
       <c r="C38" s="64"/>
       <c r="D38" s="65"/>
-      <c r="E38" s="66"/>
-      <c r="F38" s="67"/>
+      <c r="E38" s="66">
+        <v>45306</v>
+      </c>
+      <c r="F38" s="67">
+        <v>45315</v>
+      </c>
       <c r="G38" s="23"/>
-      <c r="H38" s="23" t="str">
+      <c r="H38" s="23">
         <f t="shared" si="46"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="I38" s="68"/>
       <c r="J38" s="68"/>
@@ -9038,17 +9116,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="J1:AA1"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="E3:F3"/>
     <mergeCell ref="CV4:DB4"/>
     <mergeCell ref="DC4:DI4"/>
     <mergeCell ref="BM4:BS4"/>
@@ -9056,6 +9123,17 @@
     <mergeCell ref="CA4:CG4"/>
     <mergeCell ref="CH4:CN4"/>
     <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="J1:AA1"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D13 D17:D23 D32:D59">
     <cfRule type="dataBar" priority="184">
@@ -9084,7 +9162,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;I$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="E4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>

</xml_diff>